<commit_message>
text changes in both English and French
</commit_message>
<xml_diff>
--- a/assets/files/Language_Translation.xlsx
+++ b/assets/files/Language_Translation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\mass_timber\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA6BC9AC-24D0-4EC3-9741-D964B0E7FC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC1E8D6E-3973-449D-9FCA-B859258EC831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -306,10 +306,10 @@
            A list of definitions of important building code terms is also provided for reference.
           &lt;/p&gt;
           &lt;p&gt;
-           While the Exposed Mass Timber Calculator facilitates an effective evaluation of permissible exposed mass timber elements in EMTC buildings, it is important to note that numerous other fire safety requirements must be considered in the building design. It is essential to refer to the relevant code articles to ensure compliance with these additional provisions.
+          While the Exposed Mass Timber Calculator facilitates an effective evaluation of permissible exposed mass timber elements in EMTC buildings, it is important to note that numerous other fire safety requirements must be considered in the building design. It is essential to refer to the relevant code articles to ensure compliance with these additional provisions. 
           &lt;/p&gt;
           &lt;p&gt;
-           The Exposed Mass Timber Calculator has been developed for information purposes only. Reference should always be made to the Building Code having jurisdiction. This tool should not be relied upon as a substitute for legal or design advice, and the user is responsible for how the tool is used or applied.
+           The Exposed Mass Timber Calculator has been developed for information purposes only. Reference should always be made to the Building Code having jurisdiction. This tool should not be relied upon as a substitute for legal or design advice, and the user is responsible for how the tool is used or applied. 
           &lt;/p&gt;
           &lt;p&gt;
            We appreciate any feedback or questions that you may have regarding The Exposed Mass Timber Calculator. Please email us via our helpdesk at &lt;a href='https://cwc.ca' target='_blank'&gt;cwc.ca&lt;/a&gt;.
@@ -363,10 +363,10 @@
            Une liste de définitions des termes importants du CNB est également fournie à titre de référence.
           &lt;/p&gt;
           &lt;p&gt;
-           Bien que le Calculateur debois d'oeuvre massif exposé facilite une évaluation efficace des éléments en bois d'oeuvre massif exposés admissibles dans les bâtiments CBOME, il est important de noter que de nombreuses autres exigences de sécurité incendie doivent être prises en compte dans la conception du bâtiment. Il est essentiel de se référer aux articles pertinents du code pour garantir la conformité à ces dispositions supplémentaires.
+           Bien que le Calculateur debois d'oeuvre massif exposé facilite une évaluation efficace des éléments en bois d'oeuvre massif exposés admissibles dans les bâtiments CBOME, il est important de noter que de nombreuses autres exigences de sécurité incendie doivent être prises en compte dans la conception du bâtiment. Il est essentiel de se référer aux articles pertinents du code pour garantir la conformité à ces dispositions supplémentaires. 
           &lt;/p&gt;
           &lt;p&gt;
-           Le Calculateur de bois d'oeuvre massif exposé a été développé à des fins d'information uniquement. Il convient toujours de se référer au Code du bâtiment ayant juridiction. Cet outil ne doit pas être considéré comme un substitut aux conseils juridiques ou de conception, et l'utilisateur est responsable de la manière dont l'outil est utilisé ou appliqué.
+          Le Calculateur de bois d'oeuvre massif exposé a été développé à des fins d'information uniquement. Il convient toujours de se référer au Code du bâtiment ayant juridiction. Cet outil ne doit pas être considéré comme un substitut aux conseils juridiques ou de conception, et l'utilisateur est responsable de la manière dont l'outil est utilisé ou appliqué.
           &lt;/p&gt;
           &lt;p&gt;
            Nous apprécions tous les commentaires ou questions que vous pourriez avoir concernant le Calculateur de bois d'oeuvre massif exposé. Veuillez nous envoyer un courriel via notre service d'assistance à &lt;a href='https://cwc.ca' target='_blank'&gt;cwc.ca&lt;/a&gt;.
@@ -1511,7 +1511,7 @@
               While the Exposed Mass Timber Calculator facilitates an effective evaluation of permissible exposed mass timber elements in EMTC buildings, it is important to note that numerous other fire safety requirements must be considered in the building design. It is essential to refer to the relevant code articles to ensure compliance with these additional provisions.
              &lt;/p&gt;
              &lt;p&gt;
-              While the Exposed Mass Timber Calculator facilitates an effective evaluation of permissible exposed mass timber elements in EMTC buildings, it has been developed for information purposes only. Reference should always be made to the Building Code having jurisdiction. This tool should not be relied upon as a substitute for legal or design advice, and the user is responsible for how the tool is used or applied.
+              The Exposed Mass Timber Calculator has been developed for information purposes only. Reference should always be made to the Building Code having jurisdiction. This tool should not be relied upon as a substitute for legal or design advice, and the user is responsible for how the tool is used or applied. 
              &lt;/p&gt;
 &lt;p&gt;
 Also, it is important to note that numerous other fire safety requirements must be considered in the building design. It is essential to refer to the relevant code articles to ensure compliance with these additional provisions.
@@ -1568,10 +1568,10 @@
            Une liste de définitions des termes importants du CNB est également fournie à titre de référence.
           &lt;/p&gt;
           &lt;p&gt;
-           Bien que le Calculateur debois d'oeuvre massif exposé facilite une évaluation efficace des éléments en bois d'oeuvre massif exposés admissibles dans les bâtiments CBOME, il est important de noter que de nombreuses autres exigences de sécurité incendie doivent être prises en compte dans la conception du bâtiment. Il est essentiel de se référer aux articles pertinents du code pour garantir la conformité à ces dispositions supplémentaires.
+           Bien que le Calculateur debois d'oeuvre massif exposé facilite une évaluation efficace des éléments en bois d'oeuvre massif exposés admissibles dans les bâtiments CBOME, il est important de noter que de nombreuses autres exigences de sécurité incendie doivent être prises en compte dans la conception du bâtiment. Il est essentiel de se référer aux articles pertinents du code pour garantir la conformité à ces dispositions supplémentaires. 
           &lt;/p&gt;
           &lt;p&gt;
- Bien que le Calculateur de bois d'oeuvre massif exposé facilite une évaluation efficace des éléments en bois massif exposés permis dans les bâtiments CBOME, il a été développé à des fins d'information uniquement. Il convient toujours de se référer au Code du bâtiment ayant juridiction. Cet outil ne doit pas être utilisé comme substitut aux conseils juridiques ou de conception, et l'utilisateur est responsable de la manière dont l'outil est utilisé ou appliqué.
+ Le Calculateur de bois d'oeuvre massif exposé a été développé à des fins d'information uniquement. Il convient toujours de se référer au Code du bâtiment ayant juridiction. Cet outil ne doit pas être considéré comme un substitut aux conseils juridiques ou de conception, et l'utilisateur est responsable de la manière dont l'outil est utilisé ou appliqué. 
           &lt;/p&gt;
           &lt;p&gt;
  De plus, il est important de noter que de nombreuses autres exigences de sécurité incendie doivent être prises en compte dans la conception du bâtiment. Il est essentiel de se référer aux articles pertinents du Code pour garantir la conformité à ces dispositions supplémentaires.
@@ -5677,8 +5677,8 @@
   <dimension ref="A1:F355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5924,7 +5924,7 @@
         <v>45728</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="409.5">
+    <row r="17" spans="1:5" ht="409.6">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="345">
+    <row r="20" spans="1:5" ht="336">
       <c r="A20" s="2" t="s">
         <v>77</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="409.5">
+    <row r="87" spans="1:6" ht="409.6">
       <c r="A87" s="2" t="s">
         <v>334</v>
       </c>

</xml_diff>

<commit_message>
language implementation on menu, and general fixes
</commit_message>
<xml_diff>
--- a/assets/files/Language_Translation.xlsx
+++ b/assets/files/Language_Translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\mass_timber\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF4E9C8A-6EB2-4A07-8917-ADB5EB431498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA6841B5-6438-4E22-B4DB-EF227FAA646A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="1314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="1455">
   <si>
     <t>Location (Information purposes only)</t>
   </si>
@@ -5078,6 +5078,431 @@
   </si>
   <si>
     <t>Cette fonctionnalité n'est pas disponible sur les appareils mobiles.&lt;br&gt;Veuillez utiliser un navigateur sur ordinateur.</t>
+  </si>
+  <si>
+    <t>Menu Navigation - Resources</t>
+  </si>
+  <si>
+    <t>menu_resources</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>Ressources</t>
+  </si>
+  <si>
+    <t>menu_browse_resources</t>
+  </si>
+  <si>
+    <t>Browse Resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parcourir les ressources                                            </t>
+  </si>
+  <si>
+    <t>menu_browse_resources_desc</t>
+  </si>
+  <si>
+    <t>Access a wide range of publications, solutions, and professional help to support every stage of your wood construction projects.</t>
+  </si>
+  <si>
+    <t>Accédez à un large éventail de publications, de solutions et d'aide professionnelle pour soutenir chaque étape de vos projets de construction en bois.</t>
+  </si>
+  <si>
+    <t>menu_design_tools</t>
+  </si>
+  <si>
+    <t>Design Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outils de conception                                            </t>
+  </si>
+  <si>
+    <t>menu_design_tools_desc</t>
+  </si>
+  <si>
+    <t>Certified Tools and Calculators to help you design efficient and sustainable wood structures with confidence and safety.</t>
+  </si>
+  <si>
+    <t>Outils et calculateurs certifiés pour vous aider à concevoir des structures en bois efficaces et durables en toute confiance et sécurité.</t>
+  </si>
+  <si>
+    <t>menu_elearning</t>
+  </si>
+  <si>
+    <t>eLearning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apprentissage en ligne                                            </t>
+  </si>
+  <si>
+    <t>menu_elearning_desc</t>
+  </si>
+  <si>
+    <t>Build your expertise with online courses, workshops, and training on wood construction, standards, and best practices.</t>
+  </si>
+  <si>
+    <t>Développez votre expertise grâce à des cours en ligne, des ateliers et des formations sur la construction en bois, les normes et les meilleures pratiques.</t>
+  </si>
+  <si>
+    <t>menu_wood_innovation_network</t>
+  </si>
+  <si>
+    <t>Wood Innovation Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réseau d'innovation dans le domaine du bois                                            </t>
+  </si>
+  <si>
+    <t>menu_wood_innovation_network_desc</t>
+  </si>
+  <si>
+    <t>Connect with professionals and explore cutting-edge ideas that drive innovation in wood construction and sustainability.</t>
+  </si>
+  <si>
+    <t>Entrez en contact avec des professionnels et explorez des idées de pointe qui stimulent l'innovation dans la construction en bois et le développement durable.</t>
+  </si>
+  <si>
+    <t>footer_build_safe</t>
+  </si>
+  <si>
+    <t>Build Safe and Strong with Wood</t>
+  </si>
+  <si>
+    <t>Construisez de manière sûre et solide avec le bois.</t>
+  </si>
+  <si>
+    <t>footer_software_description</t>
+  </si>
+  <si>
+    <t>WoodWorks Software® offers precision and efficiency, enabling professionals to design safe and high-quality structures that adhere to the latest Canadian building regulations.</t>
+  </si>
+  <si>
+    <t>Logiciel WoodWorks offre précision et efficacité, permettant
+aux professionnels de concevoir des structures sûres et de haute qualité qui respectent les
+dernières réglementations canadiennes en matière de construction.</t>
+  </si>
+  <si>
+    <t>footer_learn_more</t>
+  </si>
+  <si>
+    <t>Learn More</t>
+  </si>
+  <si>
+    <t>Apprendre encore plus</t>
+  </si>
+  <si>
+    <t>menu_building_with_wood</t>
+  </si>
+  <si>
+    <t>Building with Wood</t>
+  </si>
+  <si>
+    <t>Construire avec du bois</t>
+  </si>
+  <si>
+    <t>menu_why_wood_faq</t>
+  </si>
+  <si>
+    <t>Why Wood (FAQ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pourquoi le bois (FAQ)                                            </t>
+  </si>
+  <si>
+    <t>menu_wood_products</t>
+  </si>
+  <si>
+    <t>Wood Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produits du bois                                            </t>
+  </si>
+  <si>
+    <t>menu_industry_news</t>
+  </si>
+  <si>
+    <t>Industry News</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nouvelles de l'industrie                                            </t>
+  </si>
+  <si>
+    <t>menu_building_systems</t>
+  </si>
+  <si>
+    <t>Building Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codes et normes                                            </t>
+  </si>
+  <si>
+    <t>menu_need_support</t>
+  </si>
+  <si>
+    <t>Need Support?</t>
+  </si>
+  <si>
+    <t>Besoin d'aide?</t>
+  </si>
+  <si>
+    <t>menu_help_desk_description</t>
+  </si>
+  <si>
+    <t>The CWC Help Desk offers a number of resources on our Member’s Products...</t>
+  </si>
+  <si>
+    <t>Le service d'assistance de la CWC et le programme WoodWorks offrent de nombreuses ressources et un soutien technique aux professionnels de la construction.</t>
+  </si>
+  <si>
+    <t>menu_get_support</t>
+  </si>
+  <si>
+    <t>Get Support ↗</t>
+  </si>
+  <si>
+    <t>Obtenir de l'aide</t>
+  </si>
+  <si>
+    <t>menu_help_desk_form</t>
+  </si>
+  <si>
+    <t>Help Desk Form</t>
+  </si>
+  <si>
+    <t>Formulaire d'assistance</t>
+  </si>
+  <si>
+    <t>menu_publications</t>
+  </si>
+  <si>
+    <t>Publications</t>
+  </si>
+  <si>
+    <t>menu_technical_books</t>
+  </si>
+  <si>
+    <t>Technical Books</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livres techniques                                            </t>
+  </si>
+  <si>
+    <t>menu_free_publications</t>
+  </si>
+  <si>
+    <t>Free Publications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publications gratuites                                            </t>
+  </si>
+  <si>
+    <t>menu_magazine</t>
+  </si>
+  <si>
+    <t>Magazine</t>
+  </si>
+  <si>
+    <t>Revue</t>
+  </si>
+  <si>
+    <t>menu_case_studies</t>
+  </si>
+  <si>
+    <t>Case Studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Études de cas                                            </t>
+  </si>
+  <si>
+    <t>menu_award_books</t>
+  </si>
+  <si>
+    <t>Award Books</t>
+  </si>
+  <si>
+    <t>Livres des prix</t>
+  </si>
+  <si>
+    <t>menu_annual_reports</t>
+  </si>
+  <si>
+    <t>Annual Reports</t>
+  </si>
+  <si>
+    <t>Rapports annuels</t>
+  </si>
+  <si>
+    <t>footer_webstore_title</t>
+  </si>
+  <si>
+    <t>Webstore</t>
+  </si>
+  <si>
+    <t>Boutique en ligne</t>
+  </si>
+  <si>
+    <t>footer_webstore_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Découvrez des ressources essentielles pour la construction et la conception en bois. </t>
+  </si>
+  <si>
+    <t>button_access_resources</t>
+  </si>
+  <si>
+    <t>Access Resources</t>
+  </si>
+  <si>
+    <t>Accéder aux ressources</t>
+  </si>
+  <si>
+    <t>button_free_publications</t>
+  </si>
+  <si>
+    <t>Free publications</t>
+  </si>
+  <si>
+    <t>Publications gratuites</t>
+  </si>
+  <si>
+    <t>menu_events</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Événements</t>
+  </si>
+  <si>
+    <t>submenu_about_us_title</t>
+  </si>
+  <si>
+    <t>About Us</t>
+  </si>
+  <si>
+    <t>À propos de nous</t>
+  </si>
+  <si>
+    <t>submenu_about_us_desc</t>
+  </si>
+  <si>
+    <t>Learn more about our mission, team, and work.</t>
+  </si>
+  <si>
+    <t>En savoir plus sur notre mission, notre équipe et notre travail.</t>
+  </si>
+  <si>
+    <t>submenu_our_board_title</t>
+  </si>
+  <si>
+    <t>Our Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notre Conseil                                            </t>
+  </si>
+  <si>
+    <t>submenu_our_board_desc</t>
+  </si>
+  <si>
+    <t>Get to know the leaders guiding our organization.</t>
+  </si>
+  <si>
+    <t>Faites connaissance avec les dirigeants qui guident notre organisation.</t>
+  </si>
+  <si>
+    <t>submenu_our_members_title</t>
+  </si>
+  <si>
+    <t>Our Members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nos membres                                            </t>
+  </si>
+  <si>
+    <t>submenu_our_members_desc</t>
+  </si>
+  <si>
+    <t>Meet the organizations shaping the wood-building industry.</t>
+  </si>
+  <si>
+    <t>Rencontrez les organisations qui façonnent l'industrie de la construction en bois.</t>
+  </si>
+  <si>
+    <t>submenu_careers_title</t>
+  </si>
+  <si>
+    <t>Careers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrières                                            </t>
+  </si>
+  <si>
+    <t>submenu_careers_desc</t>
+  </si>
+  <si>
+    <t>Explore our job openings and other opportunities.</t>
+  </si>
+  <si>
+    <t>Découvrez nos offres d'emploi et autres opportunités.</t>
+  </si>
+  <si>
+    <t>menu_contact</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>contact_us_title</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contactez-nous                                            </t>
+  </si>
+  <si>
+    <t>contact_us_desc</t>
+  </si>
+  <si>
+    <t>Get in touch with our team...</t>
+  </si>
+  <si>
+    <t>Contactez notre équipe pour toute question, commentaire ou assistance concernant les ressources et services liés à la construction en bois.</t>
+  </si>
+  <si>
+    <t>help_desk_form_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulaire d'assistance                                            </t>
+  </si>
+  <si>
+    <t>help_desk_form_desc</t>
+  </si>
+  <si>
+    <t>Submit your questions or technical issues through our Help Desk. Our team is here to assist you.</t>
+  </si>
+  <si>
+    <t>Soumettez vos questions ou problèmes techniques par l'intermédiaire de notre service d'assistance. Notre équipe est là pour vous aider</t>
+  </si>
+  <si>
+    <t>about us menu</t>
+  </si>
+  <si>
+    <t>menu_about</t>
+  </si>
+  <si>
+    <t>codes standards</t>
+  </si>
+  <si>
+    <t>menu_codes_standards</t>
+  </si>
+  <si>
+    <t>Codes &amp; Standards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systèmes de construction                                            </t>
   </si>
   <si>
     <t>Format instructions</t>
@@ -5686,11 +6111,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F356"/>
+  <dimension ref="A1:F404"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A346" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A357" sqref="A357:A358"/>
+      <pane ySplit="1" topLeftCell="A390" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D404" sqref="D403:D404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7255,7 +7680,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="30">
+    <row r="99" spans="1:4" ht="30.75">
       <c r="A99" s="2" t="s">
         <v>381</v>
       </c>
@@ -11241,6 +11666,816 @@
       </c>
       <c r="F356" s="4">
         <v>45863</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6">
+      <c r="A357" s="2" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B357" s="2" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D357" s="7" t="s">
+        <v>1300</v>
+      </c>
+      <c r="F357" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6">
+      <c r="A358" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B358" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C358" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D358" s="7" t="s">
+        <v>1303</v>
+      </c>
+      <c r="F358" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" ht="30.75">
+      <c r="A359" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B359" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D359" s="7" t="s">
+        <v>1306</v>
+      </c>
+      <c r="F359" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6">
+      <c r="A360" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B360" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D360" s="7" t="s">
+        <v>1309</v>
+      </c>
+      <c r="F360" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" ht="30.75">
+      <c r="A361" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B361" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D361" s="7" t="s">
+        <v>1312</v>
+      </c>
+      <c r="F361" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6">
+      <c r="A362" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B362" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C362" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D362" s="7" t="s">
+        <v>1315</v>
+      </c>
+      <c r="F362" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" ht="30.75">
+      <c r="A363" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B363" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C363" s="2" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D363" s="7" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F363" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6">
+      <c r="A364" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B364" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C364" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D364" s="7" t="s">
+        <v>1321</v>
+      </c>
+      <c r="F364" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" ht="30.75">
+      <c r="A365" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B365" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C365" s="2" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D365" s="7" t="s">
+        <v>1324</v>
+      </c>
+      <c r="F365" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6">
+      <c r="A366" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B366" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C366" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D366" s="7" t="s">
+        <v>1327</v>
+      </c>
+      <c r="F366" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" ht="45.75">
+      <c r="A367" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B367" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C367" s="2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D367" s="7" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F367" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6">
+      <c r="A368" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B368" s="2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D368" s="7" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F368" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6">
+      <c r="A369" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B369" s="2" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C369" t="s">
+        <v>1335</v>
+      </c>
+      <c r="D369" s="7" t="s">
+        <v>1336</v>
+      </c>
+      <c r="F369" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6">
+      <c r="A370" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B370" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C370" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D370" s="7" t="s">
+        <v>1339</v>
+      </c>
+      <c r="F370" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6">
+      <c r="A371" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B371" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C371" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D371" s="7" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F371" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6">
+      <c r="A372" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B372" s="2" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C372" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D372" s="7" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F372" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6">
+      <c r="A373" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B373" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C373" t="s">
+        <v>1347</v>
+      </c>
+      <c r="D373" s="7" t="s">
+        <v>1348</v>
+      </c>
+      <c r="F373" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6">
+      <c r="A374" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B374" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C374" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D374" s="7" t="s">
+        <v>1351</v>
+      </c>
+      <c r="F374" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" ht="30.75">
+      <c r="A375" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B375" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C375" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D375" s="7" t="s">
+        <v>1354</v>
+      </c>
+      <c r="F375" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6">
+      <c r="A376" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B376" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C376" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D376" s="7" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F376" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6">
+      <c r="A377" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B377" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C377" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D377" s="7" t="s">
+        <v>1360</v>
+      </c>
+      <c r="F377" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6">
+      <c r="A378" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B378" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C378" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D378" s="7" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F378" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6">
+      <c r="A379" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B379" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C379" t="s">
+        <v>1364</v>
+      </c>
+      <c r="D379" s="7" t="s">
+        <v>1365</v>
+      </c>
+      <c r="F379" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6">
+      <c r="A380" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B380" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C380" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D380" s="7" t="s">
+        <v>1368</v>
+      </c>
+      <c r="F380" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6">
+      <c r="A381" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B381" s="2" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C381" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D381" s="7" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F381" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6">
+      <c r="A382" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B382" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C382" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D382" s="7" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F382" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6">
+      <c r="A383" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B383" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C383" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D383" s="7" t="s">
+        <v>1377</v>
+      </c>
+      <c r="F383" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6">
+      <c r="A384" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B384" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C384" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D384" s="7" t="s">
+        <v>1380</v>
+      </c>
+      <c r="F384" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6">
+      <c r="A385" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B385" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C385" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D385" s="7" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F385" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6">
+      <c r="A386" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B386" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C386" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D386" s="7" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F386" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6">
+      <c r="A387" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B387" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C387" t="s">
+        <v>1387</v>
+      </c>
+      <c r="D387" s="7" t="s">
+        <v>1388</v>
+      </c>
+      <c r="F387" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6">
+      <c r="A388" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B388" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C388" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D388" s="7" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F388" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6">
+      <c r="A389" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B389" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C389" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D389" s="7" t="s">
+        <v>1394</v>
+      </c>
+      <c r="F389" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6">
+      <c r="A390" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B390" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C390" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D390" s="7" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F390" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6">
+      <c r="A391" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B391" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C391" t="s">
+        <v>1399</v>
+      </c>
+      <c r="D391" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F391" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6">
+      <c r="A392" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B392" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C392" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D392" s="7" t="s">
+        <v>1403</v>
+      </c>
+      <c r="F392" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6">
+      <c r="A393" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B393" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C393" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D393" s="7" t="s">
+        <v>1406</v>
+      </c>
+      <c r="F393" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6">
+      <c r="A394" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B394" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C394" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D394" s="7" t="s">
+        <v>1409</v>
+      </c>
+      <c r="F394" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6">
+      <c r="A395" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B395" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C395" t="s">
+        <v>1411</v>
+      </c>
+      <c r="D395" s="7" t="s">
+        <v>1412</v>
+      </c>
+      <c r="F395" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6">
+      <c r="A396" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B396" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C396" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D396" s="7" t="s">
+        <v>1415</v>
+      </c>
+      <c r="F396" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6">
+      <c r="A397" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B397" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C397" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D397" s="7" t="s">
+        <v>1418</v>
+      </c>
+      <c r="F397" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6">
+      <c r="A398" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B398" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C398" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D398" s="7" t="s">
+        <v>1420</v>
+      </c>
+      <c r="F398" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6">
+      <c r="A399" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B399" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C399" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D399" s="7" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F399" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" ht="30.75">
+      <c r="A400" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B400" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C400" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D400" s="7" t="s">
+        <v>1426</v>
+      </c>
+      <c r="F400" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6">
+      <c r="A401" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B401" s="2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C401" s="2" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D401" s="7" t="s">
+        <v>1428</v>
+      </c>
+      <c r="F401" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" ht="30.75">
+      <c r="A402" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B402" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C402" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D402" s="7" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F402" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6">
+      <c r="A403" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B403" s="2" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D403" s="12" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6">
+      <c r="A404" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B404" s="2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C404" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D404" s="7" t="s">
+        <v>1437</v>
       </c>
     </row>
   </sheetData>
@@ -11269,47 +12504,47 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>1297</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>1298</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>1299</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>1300</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>1301</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>1302</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>1303</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="2" t="s">
-        <v>1304</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="3" t="s">
-        <v>1305</v>
+        <v>1446</v>
       </c>
     </row>
   </sheetData>
@@ -11340,42 +12575,42 @@
     <row r="6" spans="4:4" ht="15.75" thickBot="1"/>
     <row r="7" spans="4:4" s="13" customFormat="1" ht="37.9" customHeight="1" thickBot="1">
       <c r="D7" s="14" t="s">
-        <v>1306</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="8" spans="4:4" ht="31.15" customHeight="1">
       <c r="D8" s="15" t="s">
-        <v>1307</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="9" spans="4:4" ht="31.15" customHeight="1">
       <c r="D9" s="16" t="s">
-        <v>1308</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="10" spans="4:4" ht="31.15" customHeight="1">
       <c r="D10" s="16" t="s">
-        <v>1309</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="11" spans="4:4" ht="31.15" customHeight="1">
       <c r="D11" s="16" t="s">
-        <v>1310</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="12" spans="4:4" ht="31.15" customHeight="1">
       <c r="D12" s="16" t="s">
-        <v>1311</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="13" spans="4:4" ht="31.15" customHeight="1">
       <c r="D13" s="16" t="s">
-        <v>1312</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="14" spans="4:4" ht="22.15" customHeight="1" thickBot="1">
       <c r="D14" s="17" t="s">
-        <v>1313</v>
+        <v>1454</v>
       </c>
     </row>
   </sheetData>
@@ -11387,15 +12622,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="165a71d3-e0a0-490b-84d6-e4435d601f38">
@@ -11407,7 +12633,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058C4BCF715D4AD4F91C01182295CEFC1" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1471b12c27521517e0f325006a7c1259">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="165a71d3-e0a0-490b-84d6-e4435d601f38" xmlns:ns3="01495b67-12aa-4b93-9011-f94ea5f3e05d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8a8efc0d0e28bf6a2851dcbc84f7a3d8" ns2:_="" ns3:_="">
     <xsd:import namespace="165a71d3-e0a0-490b-84d6-e4435d601f38"/>
@@ -11674,16 +12900,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D05C45-8F4D-4FAD-AE19-B8BB44580719}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A34DC8F-73E1-4732-9E65-5077D0FB11A6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A34DC8F-73E1-4732-9E65-5077D0FB11A6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F1BB0EB-DC50-4433-BC1B-1ADF362A1D8C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F1BB0EB-DC50-4433-BC1B-1ADF362A1D8C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D05C45-8F4D-4FAD-AE19-B8BB44580719}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>